<commit_message>
more lit review completed
</commit_message>
<xml_diff>
--- a/Lit Review/Lit Review.xlsx
+++ b/Lit Review/Lit Review.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamg\Desktop\Personal\PhD Research\PhD-Research\Lit Review\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamg\Desktop\Personal\PhD Research\PhD Research\PhD\Lit Review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F0DA44-4513-4759-A552-8827E8E46C78}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F70C165D-D64F-4321-A58F-C9EB434BAF40}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{A2587338-3FF3-41C1-AB07-C709776AA103}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>Title</t>
   </si>
@@ -218,6 +218,9 @@
   </si>
   <si>
     <t>Development and Implementation of an End-Effector Upper Limb Rehabilitation Robot for Hemiplegic Patients with Line and Circle Tracking</t>
+  </si>
+  <si>
+    <t>2 or 3</t>
   </si>
 </sst>
 </file>
@@ -351,7 +354,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -368,9 +371,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -388,9 +388,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -425,6 +422,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -745,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A08E6DC-C503-4EE5-91EA-A862B24A4C16}">
   <dimension ref="B2:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,190 +777,190 @@
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="8">
-        <v>1</v>
-      </c>
-      <c r="C3" s="9" t="s">
+      <c r="B3" s="7">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="8">
-        <v>1</v>
-      </c>
-      <c r="E3" s="10">
+      <c r="D3" s="7">
+        <v>1</v>
+      </c>
+      <c r="E3" s="9">
         <v>2</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="9">
         <v>1998</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="8">
+      <c r="B4" s="7">
         <v>2</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="8">
-        <v>1</v>
-      </c>
-      <c r="E4" s="10">
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
+      <c r="E4" s="9">
         <v>2</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="9">
         <v>1993</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="3">
+      <c r="B5" s="7">
         <v>3</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="7">
         <v>2</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="9">
         <v>2</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="9">
         <v>1995</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="8">
+      <c r="B6" s="10">
         <v>4</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="8">
-        <v>1</v>
-      </c>
-      <c r="E6" s="10">
+      <c r="D6" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="12">
         <v>5</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="12">
         <v>1988</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="8">
+      <c r="B7" s="7">
         <v>5</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="8">
-        <v>1</v>
-      </c>
-      <c r="E7" s="10">
+      <c r="D7" s="7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="9">
         <v>3</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="9">
         <v>2007</v>
       </c>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="3">
+      <c r="B8" s="7">
         <v>6</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="7">
+        <v>1</v>
+      </c>
+      <c r="E8" s="7">
         <v>2</v>
       </c>
-      <c r="E8" s="3">
+      <c r="F8" s="7">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="7">
+        <v>7</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1</v>
+      </c>
+      <c r="E9" s="9">
+        <v>3</v>
+      </c>
+      <c r="F9" s="9">
+        <v>1998</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="13">
+        <v>8</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="15">
+        <v>3</v>
+      </c>
+      <c r="F10" s="15">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="7">
+        <v>9</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="7">
+        <v>1</v>
+      </c>
+      <c r="E11" s="9">
+        <v>4</v>
+      </c>
+      <c r="F11" s="9">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="10">
+        <v>10</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="10">
+        <v>3</v>
+      </c>
+      <c r="E12" s="12">
+        <v>1</v>
+      </c>
+      <c r="F12" s="12">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="13">
+        <v>11</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="13">
+        <v>5</v>
+      </c>
+      <c r="E13" s="15">
         <v>2</v>
       </c>
-      <c r="F8" s="3">
-        <v>2006</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="8">
-        <v>7</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="8">
-        <v>1</v>
-      </c>
-      <c r="E9" s="10">
-        <v>3</v>
-      </c>
-      <c r="F9" s="10">
-        <v>1998</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="11">
-        <v>8</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="14">
-        <v>3</v>
-      </c>
-      <c r="F10" s="14">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="3">
-        <v>9</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="3">
-        <v>2</v>
-      </c>
-      <c r="E11" s="2">
-        <v>3</v>
-      </c>
-      <c r="F11" s="2">
-        <v>2015</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="3">
-        <v>10</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="3">
-        <v>3</v>
-      </c>
-      <c r="E12" s="2">
-        <v>1</v>
-      </c>
-      <c r="F12" s="2">
-        <v>2008</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="15">
-        <v>11</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="15">
-        <v>5</v>
-      </c>
-      <c r="E13" s="17">
-        <v>2</v>
-      </c>
-      <c r="F13" s="17">
+      <c r="F13" s="15">
         <v>2009</v>
       </c>
     </row>
@@ -976,53 +976,53 @@
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="15">
+      <c r="B15" s="13">
         <v>13</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="13">
         <v>5</v>
       </c>
-      <c r="E15" s="17">
-        <v>1</v>
-      </c>
-      <c r="F15" s="17">
+      <c r="E15" s="15">
+        <v>1</v>
+      </c>
+      <c r="F15" s="15">
         <v>2014</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="15">
+      <c r="B16" s="13">
         <v>14</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="13">
         <v>4</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="15">
         <v>2</v>
       </c>
-      <c r="F16" s="17">
+      <c r="F16" s="15">
         <v>2004</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B17" s="8">
+      <c r="B17" s="7">
         <v>15</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="8">
-        <v>1</v>
-      </c>
-      <c r="E17" s="8">
+      <c r="D17" s="7">
+        <v>1</v>
+      </c>
+      <c r="E17" s="7">
         <v>2</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17" s="7">
         <v>2007</v>
       </c>
     </row>
@@ -1033,7 +1033,7 @@
       <c r="C18" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="7"/>
+      <c r="D18" s="6"/>
     </row>
     <row r="19" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
@@ -1044,36 +1044,36 @@
       </c>
     </row>
     <row r="20" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="18">
+      <c r="B20" s="16">
         <v>18</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D20" s="20">
+      <c r="D20" s="18">
         <v>5</v>
       </c>
-      <c r="E20" s="21">
+      <c r="E20" s="19">
         <v>3</v>
       </c>
-      <c r="F20" s="22">
+      <c r="F20" s="20">
         <v>2018</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="15">
+      <c r="B21" s="13">
         <v>19</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D21" s="15">
+      <c r="D21" s="13">
         <v>3</v>
       </c>
-      <c r="E21" s="17">
-        <v>1</v>
-      </c>
-      <c r="F21" s="17">
+      <c r="E21" s="15">
+        <v>1</v>
+      </c>
+      <c r="F21" s="15">
         <v>2013</v>
       </c>
     </row>
@@ -1102,19 +1102,19 @@
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="15">
+      <c r="B25" s="13">
         <v>23</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="C25" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="15">
+      <c r="D25" s="13">
         <v>5</v>
       </c>
-      <c r="E25" s="17">
+      <c r="E25" s="15">
         <v>3</v>
       </c>
-      <c r="F25" s="17">
+      <c r="F25" s="15">
         <v>1998</v>
       </c>
     </row>
@@ -1143,19 +1143,19 @@
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="15">
+      <c r="B29" s="13">
         <v>27</v>
       </c>
-      <c r="C29" s="16" t="s">
+      <c r="C29" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="15">
+      <c r="D29" s="13">
         <v>3</v>
       </c>
-      <c r="E29" s="17">
-        <v>1</v>
-      </c>
-      <c r="F29" s="17">
+      <c r="E29" s="15">
+        <v>1</v>
+      </c>
+      <c r="F29" s="15">
         <v>2013</v>
       </c>
     </row>
@@ -1208,19 +1208,19 @@
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="15">
+      <c r="B36" s="13">
         <v>34</v>
       </c>
-      <c r="C36" s="16" t="s">
+      <c r="C36" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="15">
+      <c r="D36" s="13">
         <v>3</v>
       </c>
-      <c r="E36" s="17">
+      <c r="E36" s="15">
         <v>3</v>
       </c>
-      <c r="F36" s="17">
+      <c r="F36" s="15">
         <v>2007</v>
       </c>
     </row>
@@ -1273,19 +1273,19 @@
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B43" s="8">
+      <c r="B43" s="7">
         <v>41</v>
       </c>
-      <c r="C43" s="9" t="s">
+      <c r="C43" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D43" s="8">
-        <v>1</v>
-      </c>
-      <c r="E43" s="10">
-        <v>1</v>
-      </c>
-      <c r="F43" s="10">
+      <c r="D43" s="7">
+        <v>1</v>
+      </c>
+      <c r="E43" s="9">
+        <v>1</v>
+      </c>
+      <c r="F43" s="9">
         <v>2005</v>
       </c>
     </row>
@@ -1300,19 +1300,19 @@
       <c r="F44" s="3"/>
     </row>
     <row r="45" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B45" s="8">
+      <c r="B45" s="7">
         <v>43</v>
       </c>
-      <c r="C45" s="9" t="s">
+      <c r="C45" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D45" s="8">
-        <v>1</v>
-      </c>
-      <c r="E45" s="8">
-        <v>1</v>
-      </c>
-      <c r="F45" s="8">
+      <c r="D45" s="7">
+        <v>1</v>
+      </c>
+      <c r="E45" s="7">
+        <v>1</v>
+      </c>
+      <c r="F45" s="7">
         <v>2002</v>
       </c>
     </row>
@@ -1327,19 +1327,19 @@
       <c r="F46" s="3"/>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B47" s="15">
+      <c r="B47" s="13">
         <v>45</v>
       </c>
-      <c r="C47" s="16" t="s">
+      <c r="C47" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D47" s="15">
+      <c r="D47" s="13">
         <v>3</v>
       </c>
-      <c r="E47" s="17">
+      <c r="E47" s="15">
         <v>2</v>
       </c>
-      <c r="F47" s="17">
+      <c r="F47" s="15">
         <v>2005</v>
       </c>
     </row>
@@ -1352,53 +1352,53 @@
       </c>
     </row>
     <row r="49" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B49" s="11">
+      <c r="B49" s="10">
         <v>47</v>
       </c>
-      <c r="C49" s="12" t="s">
+      <c r="C49" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="D49" s="11">
+      <c r="D49" s="10">
         <v>2</v>
       </c>
-      <c r="E49" s="11">
-        <v>1</v>
-      </c>
-      <c r="F49" s="11">
+      <c r="E49" s="10">
+        <v>1</v>
+      </c>
+      <c r="F49" s="10">
         <v>2008</v>
       </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B50" s="8">
+      <c r="B50" s="7">
         <v>48</v>
       </c>
-      <c r="C50" s="9" t="s">
+      <c r="C50" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D50" s="8">
-        <v>1</v>
-      </c>
-      <c r="E50" s="10">
+      <c r="D50" s="7">
+        <v>1</v>
+      </c>
+      <c r="E50" s="9">
         <v>3</v>
       </c>
-      <c r="F50" s="10">
+      <c r="F50" s="9">
         <v>2007</v>
       </c>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B51" s="15">
+      <c r="B51" s="13">
         <v>49</v>
       </c>
-      <c r="C51" s="16" t="s">
+      <c r="C51" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="D51" s="15">
+      <c r="D51" s="13">
         <v>5</v>
       </c>
-      <c r="E51" s="17">
+      <c r="E51" s="15">
         <v>2</v>
       </c>
-      <c r="F51" s="17">
+      <c r="F51" s="15">
         <v>2005</v>
       </c>
     </row>
@@ -1414,24 +1414,24 @@
       <c r="B53" s="2">
         <v>51</v>
       </c>
-      <c r="C53" s="23" t="s">
+      <c r="C53" s="21" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="54" spans="2:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="24">
+      <c r="B54" s="22">
         <v>52</v>
       </c>
-      <c r="C54" s="19" t="s">
+      <c r="C54" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="D54" s="19">
+      <c r="D54" s="17">
         <v>5</v>
       </c>
-      <c r="E54" s="19">
+      <c r="E54" s="17">
         <v>3</v>
       </c>
-      <c r="F54" s="25">
+      <c r="F54" s="23">
         <v>2017</v>
       </c>
     </row>

</xml_diff>

<commit_message>
did a shed load of work
</commit_message>
<xml_diff>
--- a/Lit Review/Lit Review.xlsx
+++ b/Lit Review/Lit Review.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamg\Desktop\Personal\PhD Research\PhD Research\PhD\Lit Review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61DD3D07-0C2D-452A-B939-29667F300D41}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA3A6206-52E0-43A7-AD9C-29C5E290CE04}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{A2587338-3FF3-41C1-AB07-C709776AA103}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Title</t>
   </si>
@@ -221,6 +221,18 @@
   </si>
   <si>
     <t>2 or 3</t>
+  </si>
+  <si>
+    <t>State of the Nation, Stroke Statistics February 2018</t>
+  </si>
+  <si>
+    <t>Spasticity after stroke. Its occurrence and association with motor impairments and activity limitations.</t>
+  </si>
+  <si>
+    <t>Neurological Principles and Rehabilitation of Action Disorders: Rehabilitation interventions</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The Science of Stroke: Mechanisms in search of Treatments</t>
   </si>
 </sst>
 </file>
@@ -740,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A08E6DC-C503-4EE5-91EA-A862B24A4C16}">
-  <dimension ref="B2:G58"/>
+  <dimension ref="B2:G82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,7 +973,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="12">
         <v>12</v>
       </c>
@@ -978,20 +990,20 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="12">
+    <row r="15" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="15">
         <v>13</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="17">
         <v>5</v>
       </c>
-      <c r="E15" s="14">
-        <v>1</v>
-      </c>
-      <c r="F15" s="14">
+      <c r="E15" s="18">
+        <v>1</v>
+      </c>
+      <c r="F15" s="19">
         <v>2014</v>
       </c>
     </row>
@@ -1479,9 +1491,177 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B58" s="2">
         <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="21">
+        <v>57</v>
+      </c>
+      <c r="C59" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D59" s="16">
+        <v>5</v>
+      </c>
+      <c r="E59" s="16">
+        <v>1</v>
+      </c>
+      <c r="F59" s="22">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="13">
+        <v>58</v>
+      </c>
+      <c r="C60" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D60" s="12">
+        <v>4</v>
+      </c>
+      <c r="E60" s="12">
+        <v>2</v>
+      </c>
+      <c r="F60" s="13">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B61" s="2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B62" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B63" s="2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B64" s="2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B65" s="13">
+        <v>63</v>
+      </c>
+      <c r="C65" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D65" s="12">
+        <v>4</v>
+      </c>
+      <c r="E65" s="12">
+        <v>3</v>
+      </c>
+      <c r="F65" s="13">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B66" s="2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B67" s="13">
+        <v>65</v>
+      </c>
+      <c r="C67" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D67" s="12">
+        <v>3</v>
+      </c>
+      <c r="E67" s="12">
+        <v>4</v>
+      </c>
+      <c r="F67" s="13">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B68" s="2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B69" s="2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B70" s="2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B71" s="2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B72" s="2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B73" s="2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B74" s="2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B75" s="2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B76" s="2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B77" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B78" s="2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B79" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B80" s="2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" s="2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82" s="2">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>